<commit_message>
Feat: Adicionar outra variável ao cálculo no Excel
</commit_message>
<xml_diff>
--- a/Transferência.xlsx
+++ b/Transferência.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jrrei\Desktop\Dev\Transferência_de_Mercadoria\Programa_Moeda_Nartic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7748D41-05D5-4906-8BFD-3ED1EA819439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC3745C0-5344-4448-8A65-79E9173E1635}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,6 +18,11 @@
     <sheet name="Plan2" sheetId="2" state="hidden" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <extLst>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -537,7 +542,7 @@
   <dimension ref="A1:B129"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -575,8 +580,12 @@
       </c>
     </row>
     <row r="5" spans="1:2" s="1" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A5" s="8"/>
-      <c r="B5" s="9"/>
+      <c r="A5" s="8">
+        <v>31407</v>
+      </c>
+      <c r="B5" s="9">
+        <v>100</v>
+      </c>
     </row>
     <row r="6" spans="1:2" s="1" customFormat="1" ht="16.5" thickBot="1">
       <c r="A6" s="8"/>

</xml_diff>